<commit_message>
Fixed Self Evaluation Protocol
</commit_message>
<xml_diff>
--- a/JS Frameworks Angular Project/JS-Frameworks-Self-Evaluation-Protocol.xlsx
+++ b/JS Frameworks Angular Project/JS-Frameworks-Self-Evaluation-Protocol.xlsx
@@ -368,10 +368,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -681,7 +681,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -691,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:E5"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -756,18 +756,18 @@
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="8" spans="2:5">
       <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="5">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>16</v>
@@ -778,9 +778,7 @@
       <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="5">
-        <v>25</v>
-      </c>
+      <c r="C9" s="5"/>
       <c r="D9" s="11" t="s">
         <v>16</v>
       </c>
@@ -1044,7 +1042,7 @@
       </c>
       <c r="C32" s="10">
         <f>SUM(C6:C31)</f>
-        <v>254</v>
+        <v>321</v>
       </c>
       <c r="D32" s="10">
         <v>330</v>

</xml_diff>